<commit_message>
Lab 3 MatStat 70%
</commit_message>
<xml_diff>
--- a/3сем/ТВиМС/Lab3/ЛР3 Критерии значимости.xlsx
+++ b/3сем/ТВиМС/Lab3/ЛР3 Критерии значимости.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>Мужчины</t>
   </si>
@@ -167,6 +167,36 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-rasch = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">t-rasch = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">t-tabl = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-tabl = </t>
+  </si>
+  <si>
+    <t>Двухвыборочный F-тест для дисперсии</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>P(F&lt;=f) одностороннее</t>
+  </si>
+  <si>
+    <t>F критическое одностороннее</t>
+  </si>
+  <si>
+    <t>Двухвыборочный t-тест с одинаковыми дисперсиями</t>
+  </si>
+  <si>
+    <t>Объединенная дисперсия</t>
   </si>
 </sst>
 </file>
@@ -265,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -285,6 +315,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -300,6 +331,125 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>20480</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>137065</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8519160" y="1211580"/>
+          <a:ext cx="3800000" cy="761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>218643</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>26534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8450580" y="2065020"/>
+          <a:ext cx="3457143" cy="1085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>110373</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>29394</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127279</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8503920" y="3417453"/>
+          <a:ext cx="5652954" cy="1853326"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -568,7 +718,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,16 +1094,16 @@
       <c r="M2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="12" t="s">
         <v>42</v>
       </c>
     </row>
@@ -997,19 +1147,19 @@
       <c r="M3" s="12">
         <v>16</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="12">
         <f>COUNT(B3:M3)</f>
         <v>12</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="12">
         <f>AVERAGE(B3:M3)</f>
         <v>73.824999999999989</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="12">
         <f>_xlfn.VAR.S(B3:M3)</f>
         <v>3388.8929545454566</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="12">
         <f>O3-1</f>
         <v>11</v>
       </c>
@@ -1054,35 +1204,259 @@
       <c r="M4" s="12">
         <v>15.7</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="12">
         <f>COUNT(B4:M4)</f>
         <v>12</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="12">
         <f>AVERAGE(B4:M4)</f>
         <v>75.75833333333334</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="12">
         <f>_xlfn.VAR.S(B4:M4)</f>
         <v>3143.264469696971</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="12">
         <f>O4-1</f>
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <f>Q3/Q4</f>
+        <v>1.0781443900812349</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <f>_xlfn.F.INV.RT(C1/2,R3,R4)</f>
+        <v>3.4736990510858088</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+    </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="Q6">
-        <f>SUM(Q3:Q4)</f>
-        <v>6532.1574242424276</v>
-      </c>
-      <c r="R6">
+      <c r="A6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <f>(P3-P4)/SQRT(Q6*(1/O3+1/O4))</f>
+        <v>-8.2864600430246044E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <f>_xlfn.T.INV.2T(C1*2,R6)</f>
+        <v>1.7171443743802424</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12">
+        <f>((R3-1)*Q3+(R4-1)*Q4)/(R3+R4-2)</f>
+        <v>3266.0787121212138</v>
+      </c>
+      <c r="R6" s="12">
         <f>SUM(R3:R4)</f>
         <v>22</v>
       </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="8">
+        <v>73.824999999999989</v>
+      </c>
+      <c r="C11" s="8">
+        <v>75.75833333333334</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="8">
+        <v>73.824999999999989</v>
+      </c>
+      <c r="H11" s="8">
+        <v>75.75833333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3388.8929545454566</v>
+      </c>
+      <c r="C12" s="8">
+        <v>3143.264469696971</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="8">
+        <v>3388.8929545454566</v>
+      </c>
+      <c r="H12" s="8">
+        <v>3143.264469696971</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="8">
+        <v>12</v>
+      </c>
+      <c r="C13" s="8">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="8">
+        <v>12</v>
+      </c>
+      <c r="H13" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="8">
+        <v>11</v>
+      </c>
+      <c r="C14" s="8">
+        <v>11</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="8">
+        <v>3266.0787121212138</v>
+      </c>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1.0781443900812349</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0.45146546272474558</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="8">
+        <v>22</v>
+      </c>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="9">
+        <v>3.4736990510858088</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="F17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="8">
+        <v>-8.2864600430246044E-2</v>
+      </c>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.46735427441534105</v>
+      </c>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="8">
+        <v>1.7171443743802424</v>
+      </c>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.93470854883068211</v>
+      </c>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="9">
+        <v>2.0738730679040258</v>
+      </c>
+      <c r="H21" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>